<commit_message>
Criando Dinamica para analise de Dashboard
</commit_message>
<xml_diff>
--- a/dashboards_I.xlsx
+++ b/dashboards_I.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Youtube/04. DashBoard Especialista/01. Dashboard 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0037237E-C88C-490F-B439-0A763663B24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44BC40C4-BABE-454A-9CDD-B13D8B786BED}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0037237E-C88C-490F-B439-0A763663B24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BE744A1-67EB-4E80-A28F-5D3ABC05F4B4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista Dados" sheetId="2" r:id="rId1"/>
     <sheet name="Dados Reservas" sheetId="3" r:id="rId2"/>
     <sheet name="Layout do Dashboard" sheetId="1" state="hidden" r:id="rId3"/>
-    <sheet name="Auxiliar" sheetId="10" r:id="rId4"/>
+    <sheet name="Dinamica" sheetId="10" r:id="rId4"/>
     <sheet name="Dashboard" sheetId="4" r:id="rId5"/>
   </sheets>
   <externalReferences>
@@ -30,6 +30,9 @@
     <definedName name="taxaComissao2">'[3]Nomes de Intervalos'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId9"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -156,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -164,11 +167,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,6 +317,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3249,6 +3372,2933 @@
 </externalLink>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Lucas Gilio Ducci" refreshedDate="45198.806474189812" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="410" xr:uid="{FB3C9785-492E-4A1A-B532-605D17392831}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Reservas"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Data" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2018-01-01T00:00:00" maxDate="2018-12-31T00:00:00"/>
+    </cacheField>
+    <cacheField name="Tipo Reserva" numFmtId="1">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Valor Total" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1345" maxValue="9845"/>
+    </cacheField>
+    <cacheField name="Vendedor" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Status" numFmtId="44">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="410">
+  <r>
+    <d v="2018-01-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1345"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1380"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1415"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3475"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1450"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1485"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2400"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1520"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1555"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1590"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1625"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1660"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1695"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1730"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1765"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1800"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1835"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-15T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5798"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1870"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1905"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-17T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2345"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1940"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1975"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2010"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2045"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2080"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2115"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2150"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2185"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2220"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2255"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2290"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2325"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-01-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2360"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-01-31T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2395"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2430"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2465"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-03T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2500"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2535"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-05T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2570"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2605"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2640"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5678"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-08T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2675"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2710"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-10T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2745"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2780"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2815"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-13T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2850"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2885"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-15T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2920"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2955"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2990"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-18T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3025"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3060"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-20T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3095"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3130"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3165"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-23T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3200"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3235"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2345"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-25T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3270"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3305"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-02-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3340"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-02-28T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3375"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-01T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1345"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1380"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1415"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1450"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5678"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="4983"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9845"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="7895"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1485"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-06T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1520"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1555"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1590"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-09T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1625"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1660"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-11T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1695"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9567"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5678"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="8765"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9456"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="4567"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1730"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1765"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-14T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1800"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1835"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-16T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1870"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1905"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1940"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-19T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1975"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2010"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-21T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2045"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2080"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2115"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-24T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2150"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2185"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-26T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2220"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2255"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2290"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-29T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2325"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-03-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2360"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-03-31T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2395"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2430"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2465"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2500"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2535"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2570"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2605"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="8967"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="7896"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="6543"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="8765"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9456"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2640"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2675"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2710"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2745"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2780"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2815"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2850"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2885"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2920"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2955"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2990"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3025"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3060"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3095"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3456"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="4567"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="5345"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3456"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3130"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3165"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3200"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3235"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3270"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3305"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3340"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3375"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-04-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3410"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-04-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3445"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1730"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1765"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1800"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1835"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1870"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1905"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1940"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1975"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2010"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2045"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2080"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2115"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2150"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2185"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2220"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2255"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2290"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2325"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2360"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2395"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2430"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2465"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2500"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2535"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2570"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2605"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2640"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2675"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2710"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-05-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2745"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-05-31T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2780"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2815"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2850"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-03T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2885"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2920"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-05T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2955"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2990"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3025"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-08T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3060"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3095"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-10T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3130"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3165"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3200"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-13T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3235"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3270"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-15T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3305"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3340"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3375"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-18T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3410"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3445"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-20T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3480"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3515"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3550"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-23T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3585"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3620"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-25T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3655"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3690"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3725"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-28T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3760"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-06-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3795"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-06-30T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3830"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1345"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1380"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1415"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3475"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1450"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1485"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2400"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1520"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1555"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1590"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1625"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1660"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1695"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1730"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1765"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1800"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1835"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-15T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5798"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1870"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1905"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-17T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2345"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1940"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1975"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2010"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2045"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2080"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2115"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2150"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2185"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2220"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2255"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2290"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2325"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-07-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2360"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-07-31T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2395"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2430"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2465"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-03T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2500"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2535"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-05T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2570"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2605"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2640"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5678"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-08T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2675"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2710"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-10T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2745"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2780"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2815"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-13T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2850"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2885"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-15T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2920"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2955"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2990"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-18T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3025"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3060"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-20T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3095"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3130"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3165"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-23T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3200"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3235"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2345"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-25T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3270"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3305"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-08-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3340"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-08-28T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3375"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-01T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1345"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1380"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1415"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1450"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5678"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="4983"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9845"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-04T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="7895"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1485"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-06T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1520"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1555"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1590"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-09T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1625"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1660"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-11T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1695"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9567"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="5678"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="8765"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9456"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="4567"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1730"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1765"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-14T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1800"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1835"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-16T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1870"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1905"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1940"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-19T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1975"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2010"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-21T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2045"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2080"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2115"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-24T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2150"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2185"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-26T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2220"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2255"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2290"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-29T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2325"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-09-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2360"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-09-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2395"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2430"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2465"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2500"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2535"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2570"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2605"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="8967"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="7896"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="6543"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="8765"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="9456"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2640"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2675"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2710"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2745"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2780"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2815"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2850"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2885"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2920"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2955"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2990"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3025"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3060"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3095"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3456"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="4567"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="5345"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3456"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3130"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3165"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3200"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3235"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3270"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3305"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3340"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3375"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-10-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3410"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-10-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3445"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1730"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1765"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-03T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1800"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1835"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-05T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="1870"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1905"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1940"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-08T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="1975"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2010"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-10T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2045"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2080"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2115"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-13T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2150"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2185"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-15T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2220"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2255"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2290"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-18T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2325"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2360"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-20T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2395"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2430"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2465"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-23T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2500"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2535"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-25T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2570"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2605"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2640"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-28T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2675"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2710"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-11-30T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2745"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-11-30T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2780"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-01T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2815"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-02T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2850"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-03T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2885"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-04T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="2920"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-05T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2955"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-06T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="2990"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-07T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3025"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-08T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3060"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-09T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3095"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-10T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3130"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-11T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3165"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-12T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3200"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-13T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3235"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-14T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3270"/>
+    <s v="Letícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-15T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3305"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-16T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3340"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-17T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3375"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-18T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3410"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-19T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3445"/>
+    <s v="Priscila"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-20T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3480"/>
+    <s v="Carlos"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-21T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3515"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-22T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3550"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-23T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3585"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-24T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3620"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-25T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3655"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-26T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3690"/>
+    <s v="Priscila"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-27T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3725"/>
+    <s v="Carlos"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-28T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3760"/>
+    <s v="Letícia"/>
+    <s v="Finalizada"/>
+  </r>
+  <r>
+    <d v="2018-12-29T00:00:00"/>
+    <s v="Serviço"/>
+    <n v="3795"/>
+    <s v="Patrícia"/>
+    <s v="Cotação"/>
+  </r>
+  <r>
+    <d v="2018-12-30T00:00:00"/>
+    <s v="Hospedagem"/>
+    <n v="3830"/>
+    <s v="Patrícia"/>
+    <s v="Finalizada"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B34B53A-E713-4624-BB96-F06A567D3CBC}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="5">
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7203CBA3-2462-4655-BF37-85939DE5172B}" name="Reservas" displayName="Reservas" ref="A2:E412">
   <autoFilter ref="A2:E412" xr:uid="{3C62A2CF-B0C6-4349-86CC-B9116E1F7234}"/>
@@ -3693,8 +6743,8 @@
   </sheetPr>
   <dimension ref="A1:E412"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10789,10 +13839,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A3:C20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10800,7 +13850,98 @@
     <col min="1" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
IMplementando Lista de Vendedores no Dashboard
</commit_message>
<xml_diff>
--- a/dashboards_I.xlsx
+++ b/dashboards_I.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/01. Dashboard 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{0037237E-C88C-490F-B439-0A763663B24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F1F86F2-6B65-4DF0-8FF8-46E270E846F9}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{0037237E-C88C-490F-B439-0A763663B24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE45C377-5DB0-4CC6-9D80-7F6280E81051}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -27,13 +27,22 @@
   <definedNames>
     <definedName name="hoteis_smart_lucro_liquido">'[1]Hotéis Smart'!$C$3:$C$9</definedName>
     <definedName name="RegrasProch">'[2]PROCV e PROCH'!$I$12:$L$13</definedName>
+    <definedName name="SegmentaçãodeDados_Vendedor">#N/A</definedName>
     <definedName name="taxaComissao2">'[3]Nomes de Intervalos'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId10"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -301,14 +310,10 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,6 +325,10 @@
     <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -3208,6 +3217,172 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Vendedor">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF0561E-8BC7-1D8B-66AB-47A8B028B870}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Vendedor"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3819525" y="1285876"/>
+              <a:ext cx="1019175" cy="1524000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa uma segmentação de dados. Segmentações de dados têm suporte no Excel 2010 ou versões posteriores.
+\Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2003 ou versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1457325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Vendedor 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B563DEDC-DA21-4146-81B2-4CE3BB3AA14B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Vendedor 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="123825" y="1857375"/>
+              <a:ext cx="1428750" cy="1524000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa uma segmentação de dados. Segmentações de dados têm suporte no Excel 2010 ou versões posteriores.
+\Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2003 ou versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -3746,7 +3921,12 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1345" maxValue="9845"/>
     </cacheField>
     <cacheField name="Vendedor" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="4">
+        <s v="Priscila"/>
+        <s v="Carlos"/>
+        <s v="Letícia"/>
+        <s v="Patrícia"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Status" numFmtId="44">
       <sharedItems count="2">
@@ -4153,7 +4333,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="2052728548"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -4165,2877 +4345,2877 @@
     <x v="0"/>
     <s v="Hospedagem"/>
     <n v="1345"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="1"/>
     <s v="Hospedagem"/>
     <n v="1380"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="2"/>
     <s v="Hospedagem"/>
     <n v="1415"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="2"/>
     <s v="Hospedagem"/>
     <n v="3475"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="3"/>
     <s v="Serviço"/>
     <n v="1450"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="4"/>
     <s v="Serviço"/>
     <n v="1485"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="4"/>
     <s v="Serviço"/>
     <n v="2400"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="5"/>
     <s v="Hospedagem"/>
     <n v="1520"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="6"/>
     <s v="Hospedagem"/>
     <n v="1555"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="7"/>
     <s v="Hospedagem"/>
     <n v="1590"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="8"/>
     <s v="Serviço"/>
     <n v="1625"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="9"/>
     <s v="Serviço"/>
     <n v="1660"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="10"/>
     <s v="Hospedagem"/>
     <n v="1695"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="11"/>
     <s v="Hospedagem"/>
     <n v="1730"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="12"/>
     <s v="Hospedagem"/>
     <n v="1765"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="13"/>
     <s v="Serviço"/>
     <n v="1800"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="14"/>
     <s v="Serviço"/>
     <n v="1835"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="14"/>
     <s v="Hospedagem"/>
     <n v="5798"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="15"/>
     <s v="Hospedagem"/>
     <n v="1870"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="16"/>
     <s v="Hospedagem"/>
     <n v="1905"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="16"/>
     <s v="Serviço"/>
     <n v="2345"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="17"/>
     <s v="Hospedagem"/>
     <n v="1940"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="18"/>
     <s v="Serviço"/>
     <n v="1975"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="19"/>
     <s v="Serviço"/>
     <n v="2010"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="20"/>
     <s v="Hospedagem"/>
     <n v="2045"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="21"/>
     <s v="Hospedagem"/>
     <n v="2080"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="22"/>
     <s v="Hospedagem"/>
     <n v="2115"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="23"/>
     <s v="Serviço"/>
     <n v="2150"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="24"/>
     <s v="Serviço"/>
     <n v="2185"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="25"/>
     <s v="Hospedagem"/>
     <n v="2220"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="26"/>
     <s v="Hospedagem"/>
     <n v="2255"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="27"/>
     <s v="Hospedagem"/>
     <n v="2290"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="28"/>
     <s v="Serviço"/>
     <n v="2325"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="29"/>
     <s v="Serviço"/>
     <n v="2360"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="30"/>
     <s v="Hospedagem"/>
     <n v="2395"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="31"/>
     <s v="Hospedagem"/>
     <n v="2430"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="32"/>
     <s v="Hospedagem"/>
     <n v="2465"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="33"/>
     <s v="Serviço"/>
     <n v="2500"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="34"/>
     <s v="Serviço"/>
     <n v="2535"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="35"/>
     <s v="Hospedagem"/>
     <n v="2570"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="36"/>
     <s v="Hospedagem"/>
     <n v="2605"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="37"/>
     <s v="Hospedagem"/>
     <n v="2640"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="37"/>
     <s v="Hospedagem"/>
     <n v="5678"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="38"/>
     <s v="Serviço"/>
     <n v="2675"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="39"/>
     <s v="Serviço"/>
     <n v="2710"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="40"/>
     <s v="Hospedagem"/>
     <n v="2745"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="41"/>
     <s v="Hospedagem"/>
     <n v="2780"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="42"/>
     <s v="Hospedagem"/>
     <n v="2815"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="43"/>
     <s v="Serviço"/>
     <n v="2850"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="44"/>
     <s v="Serviço"/>
     <n v="2885"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="45"/>
     <s v="Hospedagem"/>
     <n v="2920"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="46"/>
     <s v="Hospedagem"/>
     <n v="2955"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="47"/>
     <s v="Hospedagem"/>
     <n v="2990"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="48"/>
     <s v="Serviço"/>
     <n v="3025"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="49"/>
     <s v="Serviço"/>
     <n v="3060"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="50"/>
     <s v="Hospedagem"/>
     <n v="3095"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="51"/>
     <s v="Hospedagem"/>
     <n v="3130"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="52"/>
     <s v="Hospedagem"/>
     <n v="3165"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="53"/>
     <s v="Serviço"/>
     <n v="3200"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="54"/>
     <s v="Serviço"/>
     <n v="3235"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="54"/>
     <s v="Serviço"/>
     <n v="2345"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="55"/>
     <s v="Hospedagem"/>
     <n v="3270"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="56"/>
     <s v="Hospedagem"/>
     <n v="3305"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="57"/>
     <s v="Hospedagem"/>
     <n v="3340"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="58"/>
     <s v="Serviço"/>
     <n v="3375"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="59"/>
     <s v="Serviço"/>
     <n v="1345"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="60"/>
     <s v="Hospedagem"/>
     <n v="1380"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="61"/>
     <s v="Hospedagem"/>
     <n v="1415"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="62"/>
     <s v="Hospedagem"/>
     <n v="1450"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="62"/>
     <s v="Hospedagem"/>
     <n v="5678"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="62"/>
     <s v="Hospedagem"/>
     <n v="4983"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="62"/>
     <s v="Hospedagem"/>
     <n v="9845"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="62"/>
     <s v="Hospedagem"/>
     <n v="7895"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="63"/>
     <s v="Serviço"/>
     <n v="1485"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="64"/>
     <s v="Serviço"/>
     <n v="1520"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="65"/>
     <s v="Hospedagem"/>
     <n v="1555"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="66"/>
     <s v="Hospedagem"/>
     <n v="1590"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="67"/>
     <s v="Hospedagem"/>
     <n v="1625"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="68"/>
     <s v="Serviço"/>
     <n v="1660"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="69"/>
     <s v="Serviço"/>
     <n v="1695"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="69"/>
     <s v="Hospedagem"/>
     <n v="9567"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="69"/>
     <s v="Hospedagem"/>
     <n v="5678"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="69"/>
     <s v="Hospedagem"/>
     <n v="8765"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="69"/>
     <s v="Hospedagem"/>
     <n v="9456"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="69"/>
     <s v="Hospedagem"/>
     <n v="4567"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="70"/>
     <s v="Hospedagem"/>
     <n v="1730"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="71"/>
     <s v="Hospedagem"/>
     <n v="1765"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="72"/>
     <s v="Hospedagem"/>
     <n v="1800"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="73"/>
     <s v="Serviço"/>
     <n v="1835"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="74"/>
     <s v="Serviço"/>
     <n v="1870"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="75"/>
     <s v="Hospedagem"/>
     <n v="1905"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="76"/>
     <s v="Hospedagem"/>
     <n v="1940"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="77"/>
     <s v="Hospedagem"/>
     <n v="1975"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="78"/>
     <s v="Serviço"/>
     <n v="2010"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="79"/>
     <s v="Serviço"/>
     <n v="2045"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="80"/>
     <s v="Hospedagem"/>
     <n v="2080"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="81"/>
     <s v="Hospedagem"/>
     <n v="2115"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="82"/>
     <s v="Hospedagem"/>
     <n v="2150"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="83"/>
     <s v="Serviço"/>
     <n v="2185"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="84"/>
     <s v="Serviço"/>
     <n v="2220"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="85"/>
     <s v="Hospedagem"/>
     <n v="2255"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="86"/>
     <s v="Hospedagem"/>
     <n v="2290"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="87"/>
     <s v="Hospedagem"/>
     <n v="2325"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="88"/>
     <s v="Serviço"/>
     <n v="2360"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="89"/>
     <s v="Serviço"/>
     <n v="2395"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="90"/>
     <s v="Hospedagem"/>
     <n v="2430"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="91"/>
     <s v="Hospedagem"/>
     <n v="2465"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="92"/>
     <s v="Hospedagem"/>
     <n v="2500"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="93"/>
     <s v="Serviço"/>
     <n v="2535"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="94"/>
     <s v="Serviço"/>
     <n v="2570"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="95"/>
     <s v="Hospedagem"/>
     <n v="2605"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="95"/>
     <s v="Hospedagem"/>
     <n v="8967"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="95"/>
     <s v="Hospedagem"/>
     <n v="7896"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="95"/>
     <s v="Hospedagem"/>
     <n v="6543"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="95"/>
     <s v="Hospedagem"/>
     <n v="8765"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="95"/>
     <s v="Hospedagem"/>
     <n v="9456"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="96"/>
     <s v="Hospedagem"/>
     <n v="2640"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="97"/>
     <s v="Hospedagem"/>
     <n v="2675"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="98"/>
     <s v="Serviço"/>
     <n v="2710"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="99"/>
     <s v="Serviço"/>
     <n v="2745"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="100"/>
     <s v="Hospedagem"/>
     <n v="2780"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="101"/>
     <s v="Hospedagem"/>
     <n v="2815"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="102"/>
     <s v="Hospedagem"/>
     <n v="2850"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="103"/>
     <s v="Serviço"/>
     <n v="2885"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="104"/>
     <s v="Serviço"/>
     <n v="2920"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="105"/>
     <s v="Hospedagem"/>
     <n v="2955"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="106"/>
     <s v="Hospedagem"/>
     <n v="2990"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="107"/>
     <s v="Hospedagem"/>
     <n v="3025"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="108"/>
     <s v="Serviço"/>
     <n v="3060"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="109"/>
     <s v="Serviço"/>
     <n v="3095"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="109"/>
     <s v="Serviço"/>
     <n v="3456"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="109"/>
     <s v="Serviço"/>
     <n v="4567"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="109"/>
     <s v="Serviço"/>
     <n v="5345"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="109"/>
     <s v="Serviço"/>
     <n v="3456"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="110"/>
     <s v="Hospedagem"/>
     <n v="3130"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="111"/>
     <s v="Hospedagem"/>
     <n v="3165"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="112"/>
     <s v="Hospedagem"/>
     <n v="3200"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="113"/>
     <s v="Serviço"/>
     <n v="3235"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="114"/>
     <s v="Serviço"/>
     <n v="3270"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="115"/>
     <s v="Hospedagem"/>
     <n v="3305"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="116"/>
     <s v="Hospedagem"/>
     <n v="3340"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="117"/>
     <s v="Hospedagem"/>
     <n v="3375"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="118"/>
     <s v="Serviço"/>
     <n v="3410"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="119"/>
     <s v="Serviço"/>
     <n v="3445"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="120"/>
     <s v="Hospedagem"/>
     <n v="1730"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="121"/>
     <s v="Hospedagem"/>
     <n v="1765"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="122"/>
     <s v="Hospedagem"/>
     <n v="1800"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="123"/>
     <s v="Serviço"/>
     <n v="1835"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="124"/>
     <s v="Serviço"/>
     <n v="1870"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="125"/>
     <s v="Hospedagem"/>
     <n v="1905"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="126"/>
     <s v="Hospedagem"/>
     <n v="1940"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="127"/>
     <s v="Hospedagem"/>
     <n v="1975"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="128"/>
     <s v="Serviço"/>
     <n v="2010"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="129"/>
     <s v="Serviço"/>
     <n v="2045"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="130"/>
     <s v="Hospedagem"/>
     <n v="2080"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="131"/>
     <s v="Hospedagem"/>
     <n v="2115"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="132"/>
     <s v="Hospedagem"/>
     <n v="2150"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="133"/>
     <s v="Serviço"/>
     <n v="2185"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="134"/>
     <s v="Serviço"/>
     <n v="2220"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="135"/>
     <s v="Hospedagem"/>
     <n v="2255"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="136"/>
     <s v="Hospedagem"/>
     <n v="2290"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="137"/>
     <s v="Hospedagem"/>
     <n v="2325"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="138"/>
     <s v="Serviço"/>
     <n v="2360"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="139"/>
     <s v="Serviço"/>
     <n v="2395"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="140"/>
     <s v="Hospedagem"/>
     <n v="2430"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="141"/>
     <s v="Hospedagem"/>
     <n v="2465"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="142"/>
     <s v="Hospedagem"/>
     <n v="2500"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="143"/>
     <s v="Serviço"/>
     <n v="2535"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="144"/>
     <s v="Serviço"/>
     <n v="2570"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="145"/>
     <s v="Hospedagem"/>
     <n v="2605"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="146"/>
     <s v="Hospedagem"/>
     <n v="2640"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="147"/>
     <s v="Hospedagem"/>
     <n v="2675"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="148"/>
     <s v="Serviço"/>
     <n v="2710"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="149"/>
     <s v="Serviço"/>
     <n v="2745"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="150"/>
     <s v="Hospedagem"/>
     <n v="2780"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="151"/>
     <s v="Hospedagem"/>
     <n v="2815"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="152"/>
     <s v="Hospedagem"/>
     <n v="2850"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="153"/>
     <s v="Serviço"/>
     <n v="2885"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="154"/>
     <s v="Serviço"/>
     <n v="2920"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="155"/>
     <s v="Hospedagem"/>
     <n v="2955"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="156"/>
     <s v="Hospedagem"/>
     <n v="2990"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="157"/>
     <s v="Hospedagem"/>
     <n v="3025"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="158"/>
     <s v="Serviço"/>
     <n v="3060"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="159"/>
     <s v="Serviço"/>
     <n v="3095"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="160"/>
     <s v="Hospedagem"/>
     <n v="3130"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="161"/>
     <s v="Hospedagem"/>
     <n v="3165"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="162"/>
     <s v="Hospedagem"/>
     <n v="3200"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="163"/>
     <s v="Serviço"/>
     <n v="3235"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="164"/>
     <s v="Serviço"/>
     <n v="3270"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="165"/>
     <s v="Hospedagem"/>
     <n v="3305"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="166"/>
     <s v="Hospedagem"/>
     <n v="3340"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="167"/>
     <s v="Hospedagem"/>
     <n v="3375"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="168"/>
     <s v="Serviço"/>
     <n v="3410"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="169"/>
     <s v="Serviço"/>
     <n v="3445"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="170"/>
     <s v="Hospedagem"/>
     <n v="3480"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="171"/>
     <s v="Hospedagem"/>
     <n v="3515"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="172"/>
     <s v="Hospedagem"/>
     <n v="3550"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="173"/>
     <s v="Serviço"/>
     <n v="3585"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="174"/>
     <s v="Serviço"/>
     <n v="3620"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="175"/>
     <s v="Hospedagem"/>
     <n v="3655"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="176"/>
     <s v="Hospedagem"/>
     <n v="3690"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="177"/>
     <s v="Hospedagem"/>
     <n v="3725"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="178"/>
     <s v="Serviço"/>
     <n v="3760"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="179"/>
     <s v="Serviço"/>
     <n v="3795"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="180"/>
     <s v="Hospedagem"/>
     <n v="3830"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="181"/>
     <s v="Hospedagem"/>
     <n v="1345"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="182"/>
     <s v="Hospedagem"/>
     <n v="1380"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="183"/>
     <s v="Hospedagem"/>
     <n v="1415"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="183"/>
     <s v="Hospedagem"/>
     <n v="3475"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="184"/>
     <s v="Serviço"/>
     <n v="1450"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="185"/>
     <s v="Serviço"/>
     <n v="1485"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="185"/>
     <s v="Serviço"/>
     <n v="2400"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="186"/>
     <s v="Hospedagem"/>
     <n v="1520"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="187"/>
     <s v="Hospedagem"/>
     <n v="1555"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="188"/>
     <s v="Hospedagem"/>
     <n v="1590"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="189"/>
     <s v="Serviço"/>
     <n v="1625"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="190"/>
     <s v="Serviço"/>
     <n v="1660"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="191"/>
     <s v="Hospedagem"/>
     <n v="1695"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="192"/>
     <s v="Hospedagem"/>
     <n v="1730"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="193"/>
     <s v="Hospedagem"/>
     <n v="1765"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="194"/>
     <s v="Serviço"/>
     <n v="1800"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="195"/>
     <s v="Serviço"/>
     <n v="1835"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="195"/>
     <s v="Hospedagem"/>
     <n v="5798"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="196"/>
     <s v="Hospedagem"/>
     <n v="1870"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="197"/>
     <s v="Hospedagem"/>
     <n v="1905"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="197"/>
     <s v="Serviço"/>
     <n v="2345"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="198"/>
     <s v="Hospedagem"/>
     <n v="1940"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="199"/>
     <s v="Serviço"/>
     <n v="1975"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="200"/>
     <s v="Serviço"/>
     <n v="2010"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="201"/>
     <s v="Hospedagem"/>
     <n v="2045"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="202"/>
     <s v="Hospedagem"/>
     <n v="2080"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="203"/>
     <s v="Hospedagem"/>
     <n v="2115"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="204"/>
     <s v="Serviço"/>
     <n v="2150"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="205"/>
     <s v="Serviço"/>
     <n v="2185"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="206"/>
     <s v="Hospedagem"/>
     <n v="2220"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="207"/>
     <s v="Hospedagem"/>
     <n v="2255"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="208"/>
     <s v="Hospedagem"/>
     <n v="2290"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="209"/>
     <s v="Serviço"/>
     <n v="2325"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="210"/>
     <s v="Serviço"/>
     <n v="2360"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="211"/>
     <s v="Hospedagem"/>
     <n v="2395"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="212"/>
     <s v="Hospedagem"/>
     <n v="2430"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="213"/>
     <s v="Hospedagem"/>
     <n v="2465"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="214"/>
     <s v="Serviço"/>
     <n v="2500"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="215"/>
     <s v="Serviço"/>
     <n v="2535"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="216"/>
     <s v="Hospedagem"/>
     <n v="2570"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="217"/>
     <s v="Hospedagem"/>
     <n v="2605"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="218"/>
     <s v="Hospedagem"/>
     <n v="2640"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="218"/>
     <s v="Hospedagem"/>
     <n v="5678"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="219"/>
     <s v="Serviço"/>
     <n v="2675"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="220"/>
     <s v="Serviço"/>
     <n v="2710"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="221"/>
     <s v="Hospedagem"/>
     <n v="2745"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="222"/>
     <s v="Hospedagem"/>
     <n v="2780"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="223"/>
     <s v="Hospedagem"/>
     <n v="2815"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="224"/>
     <s v="Serviço"/>
     <n v="2850"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="225"/>
     <s v="Serviço"/>
     <n v="2885"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="226"/>
     <s v="Hospedagem"/>
     <n v="2920"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="227"/>
     <s v="Hospedagem"/>
     <n v="2955"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="228"/>
     <s v="Hospedagem"/>
     <n v="2990"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="229"/>
     <s v="Serviço"/>
     <n v="3025"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="230"/>
     <s v="Serviço"/>
     <n v="3060"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="231"/>
     <s v="Hospedagem"/>
     <n v="3095"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="232"/>
     <s v="Hospedagem"/>
     <n v="3130"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="233"/>
     <s v="Hospedagem"/>
     <n v="3165"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="234"/>
     <s v="Serviço"/>
     <n v="3200"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="235"/>
     <s v="Serviço"/>
     <n v="3235"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="235"/>
     <s v="Serviço"/>
     <n v="2345"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="236"/>
     <s v="Hospedagem"/>
     <n v="3270"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="237"/>
     <s v="Hospedagem"/>
     <n v="3305"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="238"/>
     <s v="Hospedagem"/>
     <n v="3340"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="239"/>
     <s v="Serviço"/>
     <n v="3375"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="240"/>
     <s v="Serviço"/>
     <n v="1345"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="241"/>
     <s v="Hospedagem"/>
     <n v="1380"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="242"/>
     <s v="Hospedagem"/>
     <n v="1415"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="243"/>
     <s v="Hospedagem"/>
     <n v="1450"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="243"/>
     <s v="Hospedagem"/>
     <n v="5678"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="243"/>
     <s v="Hospedagem"/>
     <n v="4983"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="243"/>
     <s v="Hospedagem"/>
     <n v="9845"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="243"/>
     <s v="Hospedagem"/>
     <n v="7895"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="244"/>
     <s v="Serviço"/>
     <n v="1485"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="245"/>
     <s v="Serviço"/>
     <n v="1520"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="246"/>
     <s v="Hospedagem"/>
     <n v="1555"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="247"/>
     <s v="Hospedagem"/>
     <n v="1590"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="248"/>
     <s v="Hospedagem"/>
     <n v="1625"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="249"/>
     <s v="Serviço"/>
     <n v="1660"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="250"/>
     <s v="Serviço"/>
     <n v="1695"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="250"/>
     <s v="Hospedagem"/>
     <n v="9567"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="250"/>
     <s v="Hospedagem"/>
     <n v="5678"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="250"/>
     <s v="Hospedagem"/>
     <n v="8765"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="250"/>
     <s v="Hospedagem"/>
     <n v="9456"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="250"/>
     <s v="Hospedagem"/>
     <n v="4567"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="251"/>
     <s v="Hospedagem"/>
     <n v="1730"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="252"/>
     <s v="Hospedagem"/>
     <n v="1765"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="253"/>
     <s v="Hospedagem"/>
     <n v="1800"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="254"/>
     <s v="Serviço"/>
     <n v="1835"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="255"/>
     <s v="Serviço"/>
     <n v="1870"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="256"/>
     <s v="Hospedagem"/>
     <n v="1905"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="257"/>
     <s v="Hospedagem"/>
     <n v="1940"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="258"/>
     <s v="Hospedagem"/>
     <n v="1975"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="259"/>
     <s v="Serviço"/>
     <n v="2010"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="260"/>
     <s v="Serviço"/>
     <n v="2045"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="261"/>
     <s v="Hospedagem"/>
     <n v="2080"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="262"/>
     <s v="Hospedagem"/>
     <n v="2115"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="263"/>
     <s v="Hospedagem"/>
     <n v="2150"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="264"/>
     <s v="Serviço"/>
     <n v="2185"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="265"/>
     <s v="Serviço"/>
     <n v="2220"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="266"/>
     <s v="Hospedagem"/>
     <n v="2255"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="267"/>
     <s v="Hospedagem"/>
     <n v="2290"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="268"/>
     <s v="Hospedagem"/>
     <n v="2325"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="269"/>
     <s v="Serviço"/>
     <n v="2360"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="269"/>
     <s v="Serviço"/>
     <n v="2395"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="270"/>
     <s v="Hospedagem"/>
     <n v="2430"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="271"/>
     <s v="Hospedagem"/>
     <n v="2465"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="272"/>
     <s v="Hospedagem"/>
     <n v="2500"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="273"/>
     <s v="Serviço"/>
     <n v="2535"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="274"/>
     <s v="Serviço"/>
     <n v="2570"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="275"/>
     <s v="Hospedagem"/>
     <n v="2605"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="275"/>
     <s v="Hospedagem"/>
     <n v="8967"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="275"/>
     <s v="Hospedagem"/>
     <n v="7896"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="275"/>
     <s v="Hospedagem"/>
     <n v="6543"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="275"/>
     <s v="Hospedagem"/>
     <n v="8765"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="275"/>
     <s v="Hospedagem"/>
     <n v="9456"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="276"/>
     <s v="Hospedagem"/>
     <n v="2640"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="277"/>
     <s v="Hospedagem"/>
     <n v="2675"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="278"/>
     <s v="Serviço"/>
     <n v="2710"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="279"/>
     <s v="Serviço"/>
     <n v="2745"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="280"/>
     <s v="Hospedagem"/>
     <n v="2780"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="281"/>
     <s v="Hospedagem"/>
     <n v="2815"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="282"/>
     <s v="Hospedagem"/>
     <n v="2850"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="283"/>
     <s v="Serviço"/>
     <n v="2885"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="284"/>
     <s v="Serviço"/>
     <n v="2920"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="285"/>
     <s v="Hospedagem"/>
     <n v="2955"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="286"/>
     <s v="Hospedagem"/>
     <n v="2990"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="287"/>
     <s v="Hospedagem"/>
     <n v="3025"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="288"/>
     <s v="Serviço"/>
     <n v="3060"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="289"/>
     <s v="Serviço"/>
     <n v="3095"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="289"/>
     <s v="Serviço"/>
     <n v="3456"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="289"/>
     <s v="Serviço"/>
     <n v="4567"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="289"/>
     <s v="Serviço"/>
     <n v="5345"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="289"/>
     <s v="Serviço"/>
     <n v="3456"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="290"/>
     <s v="Hospedagem"/>
     <n v="3130"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="291"/>
     <s v="Hospedagem"/>
     <n v="3165"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="292"/>
     <s v="Hospedagem"/>
     <n v="3200"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="293"/>
     <s v="Serviço"/>
     <n v="3235"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="294"/>
     <s v="Serviço"/>
     <n v="3270"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="295"/>
     <s v="Hospedagem"/>
     <n v="3305"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="296"/>
     <s v="Hospedagem"/>
     <n v="3340"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="297"/>
     <s v="Hospedagem"/>
     <n v="3375"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="298"/>
     <s v="Serviço"/>
     <n v="3410"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="299"/>
     <s v="Serviço"/>
     <n v="3445"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="300"/>
     <s v="Hospedagem"/>
     <n v="1730"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="301"/>
     <s v="Hospedagem"/>
     <n v="1765"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="302"/>
     <s v="Hospedagem"/>
     <n v="1800"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="303"/>
     <s v="Serviço"/>
     <n v="1835"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="304"/>
     <s v="Serviço"/>
     <n v="1870"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="305"/>
     <s v="Hospedagem"/>
     <n v="1905"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="306"/>
     <s v="Hospedagem"/>
     <n v="1940"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="307"/>
     <s v="Hospedagem"/>
     <n v="1975"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="308"/>
     <s v="Serviço"/>
     <n v="2010"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="309"/>
     <s v="Serviço"/>
     <n v="2045"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="310"/>
     <s v="Hospedagem"/>
     <n v="2080"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="311"/>
     <s v="Hospedagem"/>
     <n v="2115"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="312"/>
     <s v="Hospedagem"/>
     <n v="2150"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="313"/>
     <s v="Serviço"/>
     <n v="2185"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="314"/>
     <s v="Serviço"/>
     <n v="2220"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="315"/>
     <s v="Hospedagem"/>
     <n v="2255"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="316"/>
     <s v="Hospedagem"/>
     <n v="2290"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="317"/>
     <s v="Hospedagem"/>
     <n v="2325"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="318"/>
     <s v="Serviço"/>
     <n v="2360"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="319"/>
     <s v="Serviço"/>
     <n v="2395"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="320"/>
     <s v="Hospedagem"/>
     <n v="2430"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="321"/>
     <s v="Hospedagem"/>
     <n v="2465"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="322"/>
     <s v="Hospedagem"/>
     <n v="2500"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="323"/>
     <s v="Serviço"/>
     <n v="2535"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="324"/>
     <s v="Serviço"/>
     <n v="2570"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="325"/>
     <s v="Hospedagem"/>
     <n v="2605"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="326"/>
     <s v="Hospedagem"/>
     <n v="2640"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="327"/>
     <s v="Hospedagem"/>
     <n v="2675"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="328"/>
     <s v="Serviço"/>
     <n v="2710"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="329"/>
     <s v="Serviço"/>
     <n v="2745"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="329"/>
     <s v="Hospedagem"/>
     <n v="2780"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="330"/>
     <s v="Hospedagem"/>
     <n v="2815"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="331"/>
     <s v="Hospedagem"/>
     <n v="2850"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="332"/>
     <s v="Serviço"/>
     <n v="2885"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="333"/>
     <s v="Serviço"/>
     <n v="2920"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="334"/>
     <s v="Hospedagem"/>
     <n v="2955"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="335"/>
     <s v="Hospedagem"/>
     <n v="2990"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="336"/>
     <s v="Hospedagem"/>
     <n v="3025"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="337"/>
     <s v="Serviço"/>
     <n v="3060"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="338"/>
     <s v="Serviço"/>
     <n v="3095"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="339"/>
     <s v="Hospedagem"/>
     <n v="3130"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="340"/>
     <s v="Hospedagem"/>
     <n v="3165"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="341"/>
     <s v="Hospedagem"/>
     <n v="3200"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="342"/>
     <s v="Serviço"/>
     <n v="3235"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="343"/>
     <s v="Serviço"/>
     <n v="3270"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
     <x v="344"/>
     <s v="Hospedagem"/>
     <n v="3305"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="345"/>
     <s v="Hospedagem"/>
     <n v="3340"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="346"/>
     <s v="Hospedagem"/>
     <n v="3375"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="347"/>
     <s v="Serviço"/>
     <n v="3410"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="348"/>
     <s v="Serviço"/>
     <n v="3445"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="349"/>
     <s v="Hospedagem"/>
     <n v="3480"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="0"/>
   </r>
   <r>
     <x v="350"/>
     <s v="Hospedagem"/>
     <n v="3515"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="351"/>
     <s v="Hospedagem"/>
     <n v="3550"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="352"/>
     <s v="Serviço"/>
     <n v="3585"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
   <r>
     <x v="353"/>
     <s v="Serviço"/>
     <n v="3620"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="354"/>
     <s v="Hospedagem"/>
     <n v="3655"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="355"/>
     <s v="Hospedagem"/>
     <n v="3690"/>
-    <s v="Priscila"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <x v="356"/>
     <s v="Hospedagem"/>
     <n v="3725"/>
-    <s v="Carlos"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="357"/>
     <s v="Serviço"/>
     <n v="3760"/>
-    <s v="Letícia"/>
+    <x v="2"/>
     <x v="0"/>
   </r>
   <r>
     <x v="358"/>
     <s v="Serviço"/>
     <n v="3795"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
     <x v="359"/>
     <s v="Hospedagem"/>
     <n v="3830"/>
-    <s v="Patrícia"/>
+    <x v="3"/>
     <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B34B53A-E713-4624-BB96-F06A567D3CBC}" name="Tabela dinâmica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B34B53A-E713-4624-BB96-F06A567D3CBC}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:N9" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" numFmtId="14" showAll="0">
@@ -7405,7 +7585,15 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="44" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
         <item x="1"/>
@@ -7881,6 +8069,36 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Vendedor" xr10:uid="{781DFC0F-A422-4A25-ACCD-45DE35049F40}" sourceName="Vendedor">
+  <pivotTables>
+    <pivotTable tabId="10" name="Tabela dinâmica1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="2052728548">
+      <items count="4">
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="0" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Vendedor" xr10:uid="{FF0C0048-1D12-4C4B-8F81-A840B40D0315}" cache="SegmentaçãodeDados_Vendedor" caption="Vendedor" rowHeight="241300"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Vendedor 1" xr10:uid="{304EFDFA-2C39-48D4-8C57-7C75BE810348}" cache="SegmentaçãodeDados_Vendedor" caption="Vendedor" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7203CBA3-2462-4655-BF37-85939DE5172B}" name="Reservas" displayName="Reservas" ref="A2:E412">
   <autoFilter ref="A2:E412" xr:uid="{3C62A2CF-B0C6-4349-86CC-B9116E1F7234}"/>
@@ -8215,16 +8433,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -8325,7 +8543,7 @@
   </sheetPr>
   <dimension ref="A1:E412"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8340,13 +8558,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -15389,23 +15607,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="36" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16159,10 +16377,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16208,144 +16426,152 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="21">
         <v>22650</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="21">
         <v>31840</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="21">
         <v>24415</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="21">
         <v>35670</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="21">
         <v>27270</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="21">
         <v>39870</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="21">
         <v>22650</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="21">
         <v>31840</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="21">
         <v>24415</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="21">
         <v>35670</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="21">
         <v>27270</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="21">
         <v>39870</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="21">
         <v>363430</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="16">
+      <c r="A8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="21">
         <v>49338</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="21">
         <v>57453</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="21">
         <v>99989</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="21">
         <v>110906</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="21">
         <v>42635</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="21">
         <v>59805</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="21">
         <v>49338</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="21">
         <v>57453</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="21">
         <v>99989</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="21">
         <v>110906</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="21">
         <v>42635</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="21">
         <v>59805</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="21">
         <v>840252</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="21">
         <v>71988</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="21">
         <v>89293</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="21">
         <v>124404</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="21">
         <v>146576</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="21">
         <v>69905</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="21">
         <v>99675</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="21">
         <v>71988</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="21">
         <v>89293</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="21">
         <v>124404</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="21">
         <v>146576</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="21">
         <v>69905</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="21">
         <v>99675</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="21">
         <v>1203682</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -16357,7 +16583,7 @@
   <dimension ref="B1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16368,36 +16594,36 @@
   <sheetData>
     <row r="1" spans="2:2" ht="6" customHeight="1"/>
     <row r="2" spans="2:2" ht="21" customHeight="1">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="21" customHeight="1">
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <f>GETPIVOTDATA("Valor Total",Dinamica!$A$3)</f>
         <v>1203682</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="4.5" customHeight="1"/>
     <row r="5" spans="2:2" ht="21" customHeight="1">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="21.75" customHeight="1">
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <f>GETPIVOTDATA("Valor Total",Dinamica!$A$3,"Status","Finalizada")</f>
         <v>840252</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="4.5" customHeight="1"/>
     <row r="8" spans="2:2" ht="19.5" customHeight="1">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="21" customHeight="1">
-      <c r="B9" s="21">
+      <c r="B9" s="19">
         <f>IFERROR(B6/B3,0)</f>
         <v>0.69806809439702511</v>
       </c>
@@ -16405,5 +16631,13 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>